<commit_message>
This is the pass fail count update
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CF5690-2E14-4629-8ECC-6592155DF0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F841ED-BA9E-4A4F-B180-7ABB0C48BEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
@@ -466,12 +466,6 @@
     <t>Enter Username</t>
   </si>
   <si>
-    <t>OTP  is Display</t>
-  </si>
-  <si>
-    <t>OTP  is not Display</t>
-  </si>
-  <si>
     <t>Enter OTP</t>
   </si>
   <si>
@@ -500,6 +494,12 @@
   </si>
   <si>
     <t>tagName</t>
+  </si>
+  <si>
+    <t>mailbody  is Display</t>
+  </si>
+  <si>
+    <t>mail body   is not Display</t>
   </si>
 </sst>
 </file>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1B6DD0-F2CA-43D3-8E1C-4910C2350D51}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1190,7 +1190,7 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1465,7 +1465,7 @@
         <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1482,7 +1482,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F26" t="s">
         <v>75</v>
@@ -1563,7 +1563,7 @@
         <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>82</v>
@@ -1575,10 +1575,10 @@
         <v>94</v>
       </c>
       <c r="I30" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="J30" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="F36" s="3"/>
       <c r="H36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -1713,7 +1713,7 @@
         <v>120</v>
       </c>
       <c r="I37" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -1790,10 +1790,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
         <v>78</v>
@@ -1802,15 +1802,15 @@
         <v>79</v>
       </c>
       <c r="H41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the new HTML table
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F841ED-BA9E-4A4F-B180-7ABB0C48BEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CCE6E1-20E4-4A44-B3E9-7605A8AD679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1B6DD0-F2CA-43D3-8E1C-4910C2350D51}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1563,7 +1563,7 @@
         <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>82</v>
@@ -1595,7 +1595,7 @@
         <v>79</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Change the lattest Extent Report
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CCE6E1-20E4-4A44-B3E9-7605A8AD679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D043D3-34E3-4EAA-A28C-04A4798880F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="221">
   <si>
     <t>Si No</t>
   </si>
@@ -500,6 +501,195 @@
   </si>
   <si>
     <t>mail body   is not Display</t>
+  </si>
+  <si>
+    <t>Srno</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>PageName</t>
+  </si>
+  <si>
+    <t>RunStatus</t>
+  </si>
+  <si>
+    <t>Action_Type</t>
+  </si>
+  <si>
+    <t>Test_Case</t>
+  </si>
+  <si>
+    <t>Scenario_ID</t>
+  </si>
+  <si>
+    <t>TC_01_01</t>
+  </si>
+  <si>
+    <t>SC_01</t>
+  </si>
+  <si>
+    <t>TC_01_02</t>
+  </si>
+  <si>
+    <t>User should be able to login after entering credentials.</t>
+  </si>
+  <si>
+    <t>TC_01_03</t>
+  </si>
+  <si>
+    <t>TC_01_04</t>
+  </si>
+  <si>
+    <t>TC_01_05</t>
+  </si>
+  <si>
+    <t>SC_02</t>
+  </si>
+  <si>
+    <t>SC_03</t>
+  </si>
+  <si>
+    <t>SC_04</t>
+  </si>
+  <si>
+    <t>SC_05</t>
+  </si>
+  <si>
+    <t>SC_06</t>
+  </si>
+  <si>
+    <t>SC_07</t>
+  </si>
+  <si>
+    <t>SC_08</t>
+  </si>
+  <si>
+    <t>SC_09</t>
+  </si>
+  <si>
+    <t>SC_10</t>
+  </si>
+  <si>
+    <t>SC_11</t>
+  </si>
+  <si>
+    <t>SC_12</t>
+  </si>
+  <si>
+    <t>SC_13</t>
+  </si>
+  <si>
+    <t>SC_14</t>
+  </si>
+  <si>
+    <t>SC_15</t>
+  </si>
+  <si>
+    <t>SC_16</t>
+  </si>
+  <si>
+    <t>SC_17</t>
+  </si>
+  <si>
+    <t>SC_18</t>
+  </si>
+  <si>
+    <t>SC_19</t>
+  </si>
+  <si>
+    <t>SC_20</t>
+  </si>
+  <si>
+    <t>SC_21</t>
+  </si>
+  <si>
+    <t>SC_22</t>
+  </si>
+  <si>
+    <t>SC_23</t>
+  </si>
+  <si>
+    <t>SC_24</t>
+  </si>
+  <si>
+    <t>SC_25</t>
+  </si>
+  <si>
+    <t>SC_26</t>
+  </si>
+  <si>
+    <t>SC_27</t>
+  </si>
+  <si>
+    <t>SC_28</t>
+  </si>
+  <si>
+    <t>SC_29</t>
+  </si>
+  <si>
+    <t>SC_30</t>
+  </si>
+  <si>
+    <t>SC_31</t>
+  </si>
+  <si>
+    <t>SC_32</t>
+  </si>
+  <si>
+    <t>SC_33</t>
+  </si>
+  <si>
+    <t>SC_34</t>
+  </si>
+  <si>
+    <t>SC_35</t>
+  </si>
+  <si>
+    <t>SC_36</t>
+  </si>
+  <si>
+    <t>SC_37</t>
+  </si>
+  <si>
+    <t>SC_38</t>
+  </si>
+  <si>
+    <t>SC_39</t>
+  </si>
+  <si>
+    <t>SC_40</t>
+  </si>
+  <si>
+    <t>IshineLoginPage</t>
+  </si>
+  <si>
+    <t>MailLoginPage</t>
+  </si>
+  <si>
+    <t>MailBodyPart</t>
+  </si>
+  <si>
+    <t>IshineOTPField</t>
+  </si>
+  <si>
+    <t>Element Present or not</t>
+  </si>
+  <si>
+    <t>Handel the Window</t>
+  </si>
+  <si>
+    <t>Redirects To Ishine Login page</t>
+  </si>
+  <si>
+    <t>Redirects To Apmosys Mail Login page</t>
+  </si>
+  <si>
+    <t>User should be able to Go To mailBody And get The OTP</t>
+  </si>
+  <si>
+    <t>User should be able to login after entering OTP</t>
   </si>
 </sst>
 </file>
@@ -885,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1B6DD0-F2CA-43D3-8E1C-4910C2350D51}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1821,6 +2011,1257 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE73440-ADC0-400F-94D2-AEBDBE56EBE3}">
+  <dimension ref="A1:L41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" t="s">
+        <v>217</v>
+      </c>
+      <c r="L2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" t="s">
+        <v>217</v>
+      </c>
+      <c r="L3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" t="s">
+        <v>217</v>
+      </c>
+      <c r="L4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>215</v>
+      </c>
+      <c r="J5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K5" t="s">
+        <v>217</v>
+      </c>
+      <c r="L5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K6" t="s">
+        <v>217</v>
+      </c>
+      <c r="L6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" t="s">
+        <v>167</v>
+      </c>
+      <c r="K7" t="s">
+        <v>168</v>
+      </c>
+      <c r="L7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" t="s">
+        <v>167</v>
+      </c>
+      <c r="K8" t="s">
+        <v>168</v>
+      </c>
+      <c r="L8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" t="s">
+        <v>167</v>
+      </c>
+      <c r="K9" t="s">
+        <v>168</v>
+      </c>
+      <c r="L9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="J10" t="s">
+        <v>167</v>
+      </c>
+      <c r="K10" t="s">
+        <v>168</v>
+      </c>
+      <c r="L10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" t="s">
+        <v>167</v>
+      </c>
+      <c r="K11" t="s">
+        <v>168</v>
+      </c>
+      <c r="L11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>154</v>
+      </c>
+      <c r="J12" t="s">
+        <v>169</v>
+      </c>
+      <c r="K12" t="s">
+        <v>218</v>
+      </c>
+      <c r="L12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" t="s">
+        <v>212</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>119</v>
+      </c>
+      <c r="J13" t="s">
+        <v>169</v>
+      </c>
+      <c r="K13" t="s">
+        <v>218</v>
+      </c>
+      <c r="L13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>212</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" t="s">
+        <v>216</v>
+      </c>
+      <c r="J14" t="s">
+        <v>169</v>
+      </c>
+      <c r="K14" t="s">
+        <v>218</v>
+      </c>
+      <c r="L14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>169</v>
+      </c>
+      <c r="K15" t="s">
+        <v>218</v>
+      </c>
+      <c r="L15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" t="s">
+        <v>169</v>
+      </c>
+      <c r="K16" t="s">
+        <v>218</v>
+      </c>
+      <c r="L16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>212</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" t="s">
+        <v>169</v>
+      </c>
+      <c r="K17" t="s">
+        <v>218</v>
+      </c>
+      <c r="L17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" t="s">
+        <v>170</v>
+      </c>
+      <c r="K18" t="s">
+        <v>219</v>
+      </c>
+      <c r="L18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>212</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" t="s">
+        <v>170</v>
+      </c>
+      <c r="K19" t="s">
+        <v>219</v>
+      </c>
+      <c r="L19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>212</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" t="s">
+        <v>170</v>
+      </c>
+      <c r="K20" t="s">
+        <v>219</v>
+      </c>
+      <c r="L20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" t="s">
+        <v>170</v>
+      </c>
+      <c r="K21" t="s">
+        <v>219</v>
+      </c>
+      <c r="L21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" t="s">
+        <v>170</v>
+      </c>
+      <c r="K22" t="s">
+        <v>219</v>
+      </c>
+      <c r="L22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>212</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" t="s">
+        <v>170</v>
+      </c>
+      <c r="K23" t="s">
+        <v>219</v>
+      </c>
+      <c r="L23" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" t="s">
+        <v>212</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" t="s">
+        <v>170</v>
+      </c>
+      <c r="K24" t="s">
+        <v>219</v>
+      </c>
+      <c r="L24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>212</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>153</v>
+      </c>
+      <c r="J25" t="s">
+        <v>170</v>
+      </c>
+      <c r="K25" t="s">
+        <v>219</v>
+      </c>
+      <c r="L25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" t="s">
+        <v>76</v>
+      </c>
+      <c r="J26" t="s">
+        <v>170</v>
+      </c>
+      <c r="K26" t="s">
+        <v>219</v>
+      </c>
+      <c r="L26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>87</v>
+      </c>
+      <c r="J27" t="s">
+        <v>170</v>
+      </c>
+      <c r="K27" t="s">
+        <v>219</v>
+      </c>
+      <c r="L27" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>213</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H28" t="s">
+        <v>83</v>
+      </c>
+      <c r="J28" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28" t="s">
+        <v>219</v>
+      </c>
+      <c r="L28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="H29" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" t="s">
+        <v>170</v>
+      </c>
+      <c r="K29" t="s">
+        <v>219</v>
+      </c>
+      <c r="L29" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>213</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G30" t="s">
+        <v>93</v>
+      </c>
+      <c r="H30" t="s">
+        <v>94</v>
+      </c>
+      <c r="J30" t="s">
+        <v>170</v>
+      </c>
+      <c r="K30" t="s">
+        <v>219</v>
+      </c>
+      <c r="L30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>213</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" t="s">
+        <v>80</v>
+      </c>
+      <c r="J31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K31" t="s">
+        <v>219</v>
+      </c>
+      <c r="L31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>213</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s">
+        <v>121</v>
+      </c>
+      <c r="J32" t="s">
+        <v>170</v>
+      </c>
+      <c r="K32" t="s">
+        <v>219</v>
+      </c>
+      <c r="L32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>96</v>
+      </c>
+      <c r="J33" t="s">
+        <v>170</v>
+      </c>
+      <c r="K33" t="s">
+        <v>219</v>
+      </c>
+      <c r="L33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>213</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" t="s">
+        <v>170</v>
+      </c>
+      <c r="K34" t="s">
+        <v>219</v>
+      </c>
+      <c r="L34" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s">
+        <v>214</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>123</v>
+      </c>
+      <c r="J35" t="s">
+        <v>171</v>
+      </c>
+      <c r="K35" t="s">
+        <v>220</v>
+      </c>
+      <c r="L35" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>214</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="3"/>
+      <c r="H36" t="s">
+        <v>147</v>
+      </c>
+      <c r="J36" t="s">
+        <v>171</v>
+      </c>
+      <c r="K36" t="s">
+        <v>220</v>
+      </c>
+      <c r="L36" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>214</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H37" t="s">
+        <v>120</v>
+      </c>
+      <c r="J37" t="s">
+        <v>171</v>
+      </c>
+      <c r="K37" t="s">
+        <v>220</v>
+      </c>
+      <c r="L37" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>214</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" t="s">
+        <v>93</v>
+      </c>
+      <c r="H38" t="s">
+        <v>94</v>
+      </c>
+      <c r="J38" t="s">
+        <v>171</v>
+      </c>
+      <c r="K38" t="s">
+        <v>220</v>
+      </c>
+      <c r="L38" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>214</v>
+      </c>
+      <c r="D39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" t="s">
+        <v>72</v>
+      </c>
+      <c r="J39" t="s">
+        <v>171</v>
+      </c>
+      <c r="K39" t="s">
+        <v>220</v>
+      </c>
+      <c r="L39" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
+        <v>214</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" t="s">
+        <v>95</v>
+      </c>
+      <c r="J40" t="s">
+        <v>171</v>
+      </c>
+      <c r="K40" t="s">
+        <v>220</v>
+      </c>
+      <c r="L40" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>214</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s">
+        <v>152</v>
+      </c>
+      <c r="J41" t="s">
+        <v>171</v>
+      </c>
+      <c r="K41" t="s">
+        <v>220</v>
+      </c>
+      <c r="L41" t="s">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B700F1-826A-4855-8A91-C6D9EF1F36AA}">
   <dimension ref="A1:F2"/>
   <sheetViews>

</xml_diff>

<commit_message>
add some error print statement if the element not found and logs
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562A66A7-97F6-4A75-9880-7677F7894AB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671E513D-3051-4BDA-8E73-D53EA616ADC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
@@ -2015,7 +2015,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add the dynamic report location
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80FB27D-0F39-4396-B956-2235E2CA784C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC12487-FAEA-4E73-8D22-3D5D0F562681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="187">
   <si>
     <t>Si No</t>
   </si>
@@ -524,172 +524,70 @@
     <t>Scenario_ID</t>
   </si>
   <si>
+    <t>IshineLoginPage</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>TC_01_01</t>
   </si>
   <si>
+    <t>Redirects To Ishine Login page</t>
+  </si>
+  <si>
     <t>SC_01</t>
   </si>
   <si>
+    <t>SC_02</t>
+  </si>
+  <si>
+    <t>SC_03</t>
+  </si>
+  <si>
+    <t>SC_04</t>
+  </si>
+  <si>
+    <t>SC_05</t>
+  </si>
+  <si>
     <t>TC_01_02</t>
   </si>
   <si>
     <t>User should be able to login after entering credentials.</t>
   </si>
   <si>
-    <t>TC_01_03</t>
-  </si>
-  <si>
-    <t>TC_01_04</t>
+    <t>SC_06</t>
+  </si>
+  <si>
+    <t>SC_07</t>
+  </si>
+  <si>
+    <t>SC_08</t>
+  </si>
+  <si>
+    <t>SC_09</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Enter Username']</t>
+  </si>
+  <si>
+    <t>//input[@placeholder='Enter Password']</t>
+  </si>
+  <si>
+    <t>//button[@type='submit']</t>
+  </si>
+  <si>
+    <t>IshineOTPField</t>
   </si>
   <si>
     <t>TC_01_05</t>
   </si>
   <si>
-    <t>SC_02</t>
-  </si>
-  <si>
-    <t>SC_03</t>
-  </si>
-  <si>
-    <t>SC_04</t>
-  </si>
-  <si>
-    <t>SC_05</t>
-  </si>
-  <si>
-    <t>SC_06</t>
-  </si>
-  <si>
-    <t>SC_07</t>
-  </si>
-  <si>
-    <t>SC_08</t>
-  </si>
-  <si>
-    <t>SC_09</t>
-  </si>
-  <si>
-    <t>SC_10</t>
-  </si>
-  <si>
-    <t>SC_11</t>
-  </si>
-  <si>
-    <t>SC_12</t>
-  </si>
-  <si>
-    <t>SC_13</t>
-  </si>
-  <si>
-    <t>SC_14</t>
-  </si>
-  <si>
-    <t>SC_15</t>
-  </si>
-  <si>
-    <t>SC_16</t>
-  </si>
-  <si>
-    <t>SC_17</t>
-  </si>
-  <si>
-    <t>SC_18</t>
-  </si>
-  <si>
-    <t>SC_19</t>
-  </si>
-  <si>
-    <t>SC_20</t>
-  </si>
-  <si>
-    <t>SC_21</t>
-  </si>
-  <si>
-    <t>SC_22</t>
-  </si>
-  <si>
-    <t>SC_23</t>
-  </si>
-  <si>
-    <t>SC_24</t>
-  </si>
-  <si>
-    <t>SC_25</t>
-  </si>
-  <si>
-    <t>SC_26</t>
-  </si>
-  <si>
-    <t>SC_27</t>
-  </si>
-  <si>
-    <t>SC_28</t>
-  </si>
-  <si>
-    <t>SC_29</t>
-  </si>
-  <si>
-    <t>SC_30</t>
-  </si>
-  <si>
-    <t>SC_31</t>
-  </si>
-  <si>
-    <t>SC_32</t>
-  </si>
-  <si>
-    <t>SC_33</t>
-  </si>
-  <si>
-    <t>SC_34</t>
-  </si>
-  <si>
-    <t>SC_35</t>
-  </si>
-  <si>
-    <t>SC_36</t>
-  </si>
-  <si>
-    <t>SC_37</t>
-  </si>
-  <si>
-    <t>SC_38</t>
-  </si>
-  <si>
-    <t>SC_39</t>
+    <t>User should be able to login after entering OTP</t>
   </si>
   <si>
     <t>SC_40</t>
-  </si>
-  <si>
-    <t>IshineLoginPage</t>
-  </si>
-  <si>
-    <t>MailLoginPage</t>
-  </si>
-  <si>
-    <t>MailBodyPart</t>
-  </si>
-  <si>
-    <t>IshineOTPField</t>
-  </si>
-  <si>
-    <t>Element Present or not</t>
-  </si>
-  <si>
-    <t>Handel the Window</t>
-  </si>
-  <si>
-    <t>Redirects To Ishine Login page</t>
-  </si>
-  <si>
-    <t>Redirects To Apmosys Mail Login page</t>
-  </si>
-  <si>
-    <t>User should be able to Go To mailBody And get The OTP</t>
-  </si>
-  <si>
-    <t>User should be able to login after entering OTP</t>
   </si>
 </sst>
 </file>
@@ -2011,1257 +1909,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE73440-ADC0-400F-94D2-AEBDBE56EBE3}">
-  <dimension ref="A1:L41"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>165</v>
-      </c>
-      <c r="K2" t="s">
-        <v>217</v>
-      </c>
-      <c r="L2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" t="s">
-        <v>211</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>165</v>
-      </c>
-      <c r="K3" t="s">
-        <v>217</v>
-      </c>
-      <c r="L3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" t="s">
-        <v>165</v>
-      </c>
-      <c r="K4" t="s">
-        <v>217</v>
-      </c>
-      <c r="L4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I5" t="s">
-        <v>215</v>
-      </c>
-      <c r="J5" t="s">
-        <v>165</v>
-      </c>
-      <c r="K5" t="s">
-        <v>217</v>
-      </c>
-      <c r="L5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>89</v>
-      </c>
-      <c r="J6" t="s">
-        <v>165</v>
-      </c>
-      <c r="K6" t="s">
-        <v>217</v>
-      </c>
-      <c r="L6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>135</v>
-      </c>
-      <c r="J7" t="s">
-        <v>167</v>
-      </c>
-      <c r="K7" t="s">
-        <v>168</v>
-      </c>
-      <c r="L7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" t="s">
-        <v>91</v>
-      </c>
-      <c r="G8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" t="s">
-        <v>167</v>
-      </c>
-      <c r="K8" t="s">
-        <v>168</v>
-      </c>
-      <c r="L8" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>135</v>
-      </c>
-      <c r="J9" t="s">
-        <v>167</v>
-      </c>
-      <c r="K9" t="s">
-        <v>168</v>
-      </c>
-      <c r="L9" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H10" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" t="s">
-        <v>167</v>
-      </c>
-      <c r="K10" t="s">
-        <v>168</v>
-      </c>
-      <c r="L10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" t="s">
-        <v>211</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" t="s">
-        <v>167</v>
-      </c>
-      <c r="K11" t="s">
-        <v>168</v>
-      </c>
-      <c r="L11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" t="s">
-        <v>154</v>
-      </c>
-      <c r="J12" t="s">
-        <v>169</v>
-      </c>
-      <c r="K12" t="s">
-        <v>218</v>
-      </c>
-      <c r="L12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>212</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>119</v>
-      </c>
-      <c r="J13" t="s">
-        <v>169</v>
-      </c>
-      <c r="K13" t="s">
-        <v>218</v>
-      </c>
-      <c r="L13" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>122</v>
-      </c>
-      <c r="I14" t="s">
-        <v>216</v>
-      </c>
-      <c r="J14" t="s">
-        <v>169</v>
-      </c>
-      <c r="K14" t="s">
-        <v>218</v>
-      </c>
-      <c r="L14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" t="s">
-        <v>212</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" t="s">
-        <v>169</v>
-      </c>
-      <c r="K15" t="s">
-        <v>218</v>
-      </c>
-      <c r="L15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" t="s">
-        <v>212</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" t="s">
-        <v>95</v>
-      </c>
-      <c r="J16" t="s">
-        <v>169</v>
-      </c>
-      <c r="K16" t="s">
-        <v>218</v>
-      </c>
-      <c r="L16" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" t="s">
-        <v>212</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" t="s">
-        <v>169</v>
-      </c>
-      <c r="K17" t="s">
-        <v>218</v>
-      </c>
-      <c r="L17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" t="s">
-        <v>212</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" t="s">
-        <v>69</v>
-      </c>
-      <c r="J18" t="s">
-        <v>170</v>
-      </c>
-      <c r="K18" t="s">
-        <v>219</v>
-      </c>
-      <c r="L18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" t="s">
-        <v>212</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" t="s">
-        <v>170</v>
-      </c>
-      <c r="K19" t="s">
-        <v>219</v>
-      </c>
-      <c r="L19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s">
-        <v>212</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" t="s">
-        <v>72</v>
-      </c>
-      <c r="J20" t="s">
-        <v>170</v>
-      </c>
-      <c r="K20" t="s">
-        <v>219</v>
-      </c>
-      <c r="L20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>212</v>
-      </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>90</v>
-      </c>
-      <c r="J21" t="s">
-        <v>170</v>
-      </c>
-      <c r="K21" t="s">
-        <v>219</v>
-      </c>
-      <c r="L21" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" t="s">
-        <v>212</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" t="s">
-        <v>69</v>
-      </c>
-      <c r="J22" t="s">
-        <v>170</v>
-      </c>
-      <c r="K22" t="s">
-        <v>219</v>
-      </c>
-      <c r="L22" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>212</v>
-      </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23" t="s">
-        <v>170</v>
-      </c>
-      <c r="K23" t="s">
-        <v>219</v>
-      </c>
-      <c r="L23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" t="s">
-        <v>212</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J24" t="s">
-        <v>170</v>
-      </c>
-      <c r="K24" t="s">
-        <v>219</v>
-      </c>
-      <c r="L24" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" t="s">
-        <v>212</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" t="s">
-        <v>153</v>
-      </c>
-      <c r="J25" t="s">
-        <v>170</v>
-      </c>
-      <c r="K25" t="s">
-        <v>219</v>
-      </c>
-      <c r="L25" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" t="s">
-        <v>213</v>
-      </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" t="s">
-        <v>155</v>
-      </c>
-      <c r="F26" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" t="s">
-        <v>76</v>
-      </c>
-      <c r="J26" t="s">
-        <v>170</v>
-      </c>
-      <c r="K26" t="s">
-        <v>219</v>
-      </c>
-      <c r="L26" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>213</v>
-      </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
-        <v>87</v>
-      </c>
-      <c r="J27" t="s">
-        <v>170</v>
-      </c>
-      <c r="K27" t="s">
-        <v>219</v>
-      </c>
-      <c r="L27" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" t="s">
-        <v>213</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" t="s">
-        <v>83</v>
-      </c>
-      <c r="J28" t="s">
-        <v>170</v>
-      </c>
-      <c r="K28" t="s">
-        <v>219</v>
-      </c>
-      <c r="L28" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" t="s">
-        <v>213</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="H29" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" t="s">
-        <v>170</v>
-      </c>
-      <c r="K29" t="s">
-        <v>219</v>
-      </c>
-      <c r="L29" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" t="s">
-        <v>213</v>
-      </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G30" t="s">
-        <v>93</v>
-      </c>
-      <c r="H30" t="s">
-        <v>94</v>
-      </c>
-      <c r="J30" t="s">
-        <v>170</v>
-      </c>
-      <c r="K30" t="s">
-        <v>219</v>
-      </c>
-      <c r="L30" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>213</v>
-      </c>
-      <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H31" t="s">
-        <v>80</v>
-      </c>
-      <c r="J31" t="s">
-        <v>170</v>
-      </c>
-      <c r="K31" t="s">
-        <v>219</v>
-      </c>
-      <c r="L31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" t="s">
-        <v>213</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" t="s">
-        <v>121</v>
-      </c>
-      <c r="J32" t="s">
-        <v>170</v>
-      </c>
-      <c r="K32" t="s">
-        <v>219</v>
-      </c>
-      <c r="L32" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B33" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" t="s">
-        <v>213</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" t="s">
-        <v>96</v>
-      </c>
-      <c r="J33" t="s">
-        <v>170</v>
-      </c>
-      <c r="K33" t="s">
-        <v>219</v>
-      </c>
-      <c r="L33" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" t="s">
-        <v>213</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" t="s">
-        <v>87</v>
-      </c>
-      <c r="J34" t="s">
-        <v>170</v>
-      </c>
-      <c r="K34" t="s">
-        <v>219</v>
-      </c>
-      <c r="L34" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" t="s">
-        <v>214</v>
-      </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
-        <v>123</v>
-      </c>
-      <c r="J35" t="s">
-        <v>171</v>
-      </c>
-      <c r="K35" t="s">
-        <v>220</v>
-      </c>
-      <c r="L35" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" t="s">
-        <v>214</v>
-      </c>
-      <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="3"/>
-      <c r="H36" t="s">
-        <v>147</v>
-      </c>
-      <c r="J36" t="s">
-        <v>171</v>
-      </c>
-      <c r="K36" t="s">
-        <v>220</v>
-      </c>
-      <c r="L36" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" t="s">
-        <v>214</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H37" t="s">
-        <v>120</v>
-      </c>
-      <c r="J37" t="s">
-        <v>171</v>
-      </c>
-      <c r="K37" t="s">
-        <v>220</v>
-      </c>
-      <c r="L37" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" t="s">
-        <v>214</v>
-      </c>
-      <c r="D38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" t="s">
-        <v>92</v>
-      </c>
-      <c r="G38" t="s">
-        <v>93</v>
-      </c>
-      <c r="H38" t="s">
-        <v>94</v>
-      </c>
-      <c r="J38" t="s">
-        <v>171</v>
-      </c>
-      <c r="K38" t="s">
-        <v>220</v>
-      </c>
-      <c r="L38" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" t="s">
-        <v>214</v>
-      </c>
-      <c r="D39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
-        <v>70</v>
-      </c>
-      <c r="F39" t="s">
-        <v>92</v>
-      </c>
-      <c r="H39" t="s">
-        <v>72</v>
-      </c>
-      <c r="J39" t="s">
-        <v>171</v>
-      </c>
-      <c r="K39" t="s">
-        <v>220</v>
-      </c>
-      <c r="L39" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" t="s">
-        <v>214</v>
-      </c>
-      <c r="D40" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" t="s">
-        <v>95</v>
-      </c>
-      <c r="J40" t="s">
-        <v>171</v>
-      </c>
-      <c r="K40" t="s">
-        <v>220</v>
-      </c>
-      <c r="L40" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" t="s">
-        <v>214</v>
-      </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" t="s">
-        <v>152</v>
-      </c>
-      <c r="J41" t="s">
-        <v>171</v>
-      </c>
-      <c r="K41" t="s">
-        <v>220</v>
-      </c>
-      <c r="L41" t="s">
-        <v>210</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B700F1-826A-4855-8A91-C6D9EF1F36AA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3322,4 +1969,440 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" t="s">
+        <v>168</v>
+      </c>
+      <c r="L2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J3" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J4" t="s">
+        <v>167</v>
+      </c>
+      <c r="K4" t="s">
+        <v>168</v>
+      </c>
+      <c r="L4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J5" t="s">
+        <v>167</v>
+      </c>
+      <c r="K5" t="s">
+        <v>168</v>
+      </c>
+      <c r="L5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" t="s">
+        <v>166</v>
+      </c>
+      <c r="J6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K6" t="s">
+        <v>168</v>
+      </c>
+      <c r="L6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" t="s">
+        <v>174</v>
+      </c>
+      <c r="K7" t="s">
+        <v>175</v>
+      </c>
+      <c r="L7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" t="s">
+        <v>166</v>
+      </c>
+      <c r="J8" t="s">
+        <v>174</v>
+      </c>
+      <c r="K8" t="s">
+        <v>175</v>
+      </c>
+      <c r="L8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>166</v>
+      </c>
+      <c r="J9" t="s">
+        <v>174</v>
+      </c>
+      <c r="K9" t="s">
+        <v>175</v>
+      </c>
+      <c r="L9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10" t="s">
+        <v>174</v>
+      </c>
+      <c r="K10" t="s">
+        <v>175</v>
+      </c>
+      <c r="L10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>152</v>
+      </c>
+      <c r="J11" t="s">
+        <v>184</v>
+      </c>
+      <c r="K11" t="s">
+        <v>185</v>
+      </c>
+      <c r="L11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add try catch block properly and mail report design and report file and add the file validation properly
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC12487-FAEA-4E73-8D22-3D5D0F562681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA82A7E-4B37-4B58-8EAA-A52ACD94BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="179">
   <si>
     <t>Si No</t>
   </si>
@@ -539,36 +539,12 @@
     <t>SC_01</t>
   </si>
   <si>
-    <t>SC_02</t>
-  </si>
-  <si>
-    <t>SC_03</t>
-  </si>
-  <si>
-    <t>SC_04</t>
-  </si>
-  <si>
-    <t>SC_05</t>
-  </si>
-  <si>
     <t>TC_01_02</t>
   </si>
   <si>
     <t>User should be able to login after entering credentials.</t>
   </si>
   <si>
-    <t>SC_06</t>
-  </si>
-  <si>
-    <t>SC_07</t>
-  </si>
-  <si>
-    <t>SC_08</t>
-  </si>
-  <si>
-    <t>SC_09</t>
-  </si>
-  <si>
     <t>//input[@placeholder='Enter Username']</t>
   </si>
   <si>
@@ -581,13 +557,13 @@
     <t>IshineOTPField</t>
   </si>
   <si>
-    <t>TC_01_05</t>
-  </si>
-  <si>
     <t>User should be able to login after entering OTP</t>
   </si>
   <si>
-    <t>SC_40</t>
+    <t>TC_01_03</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -1976,7 +1952,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2106,7 +2082,7 @@
         <v>168</v>
       </c>
       <c r="L3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2144,7 +2120,7 @@
         <v>168</v>
       </c>
       <c r="L4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -2164,7 +2140,7 @@
         <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G5" t="s">
         <v>93</v>
@@ -2182,7 +2158,7 @@
         <v>168</v>
       </c>
       <c r="L5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2202,7 +2178,7 @@
         <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
@@ -2220,7 +2196,7 @@
         <v>168</v>
       </c>
       <c r="L6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -2252,13 +2228,13 @@
         <v>166</v>
       </c>
       <c r="J7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="L7" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2272,13 +2248,13 @@
         <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>178</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="G8" t="s">
         <v>22</v>
@@ -2290,13 +2266,13 @@
         <v>166</v>
       </c>
       <c r="J8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="L8" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -2313,33 +2289,33 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="G9" t="s">
-        <v>166</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="I9" t="s">
         <v>166</v>
       </c>
       <c r="J9" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K9" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="L9" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>78</v>
@@ -2354,7 +2330,7 @@
         <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="G10" t="s">
         <v>93</v>
@@ -2366,24 +2342,24 @@
         <v>166</v>
       </c>
       <c r="J10" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K10" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="L10" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>78</v>
       </c>
       <c r="C11" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -2392,13 +2368,13 @@
         <v>152</v>
       </c>
       <c r="J11" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="K11" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="L11" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
this is changes of jar file to run the jar file to jenkins
</commit_message>
<xml_diff>
--- a/DataSheet/IshinePortal.xlsx
+++ b/DataSheet/IshinePortal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa\eclipse-workspace\BiswajitFramework\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA82A7E-4B37-4B58-8EAA-A52ACD94BFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8836433B-9A2A-4F4F-BAB7-4F67EBDCC35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B5C4A126-B641-4661-957C-F82AF751E901}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="181">
   <si>
     <t>Si No</t>
   </si>
@@ -564,13 +564,19 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>1552x832</t>
+  </si>
+  <si>
+    <t>setWindowSize</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -595,6 +601,12 @@
     <font>
       <sz val="7"/>
       <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -626,12 +638,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1949,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,9 +2078,6 @@
       <c r="E3" t="s">
         <v>166</v>
       </c>
-      <c r="F3" t="s">
-        <v>166</v>
-      </c>
       <c r="G3" t="s">
         <v>85</v>
       </c>
@@ -2087,7 +2099,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>78</v>
@@ -2102,13 +2114,10 @@
         <v>166</v>
       </c>
       <c r="F4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G4" t="s">
-        <v>166</v>
-      </c>
-      <c r="H4" t="s">
-        <v>90</v>
+        <v>179</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="I4" t="s">
         <v>166</v>
@@ -2125,7 +2134,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>78</v>
@@ -2137,16 +2146,16 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>166</v>
       </c>
       <c r="F5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>166</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I5" t="s">
         <v>166</v>
@@ -2163,7 +2172,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>78</v>
@@ -2181,10 +2190,10 @@
         <v>172</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="H6" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I6" t="s">
         <v>166</v>
@@ -2201,7 +2210,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>78</v>
@@ -2213,25 +2222,25 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>21</v>
       </c>
       <c r="H7" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="I7" t="s">
         <v>166</v>
       </c>
       <c r="J7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L7" t="s">
         <v>169</v>
@@ -2239,7 +2248,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
@@ -2248,19 +2257,19 @@
         <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="F8" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>166</v>
       </c>
       <c r="H8" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="I8" t="s">
         <v>166</v>
@@ -2277,7 +2286,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>78</v>
@@ -2286,10 +2295,10 @@
         <v>165</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>178</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
         <v>173</v>
@@ -2315,7 +2324,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>78</v>
@@ -2330,13 +2339,13 @@
         <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I10" t="s">
         <v>166</v>
@@ -2353,27 +2362,65 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J11" t="s">
+        <v>170</v>
+      </c>
+      <c r="K11" t="s">
+        <v>171</v>
+      </c>
+      <c r="L11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
         <v>175</v>
       </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>152</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" t="s">
         <v>177</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>176</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>